<commit_message>
Removed the incognito mode from chrome open browser activity
</commit_message>
<xml_diff>
--- a/Data/Input/InputAddresses.xlsx
+++ b/Data/Input/InputAddresses.xlsx
@@ -36,19 +36,19 @@
     <x:t>320 Pitt Street, Sydney, 2000</x:t>
   </x:si>
   <x:si>
-    <x:t>210325.014942_Success</x:t>
+    <x:t>210329.035508_Success</x:t>
   </x:si>
   <x:si>
     <x:t>123 Pitt Street, Sydney, NSW</x:t>
   </x:si>
   <x:si>
-    <x:t>210325.014953_Success</x:t>
+    <x:t>210329.035519_Success</x:t>
   </x:si>
   <x:si>
     <x:t>555 Anzac Parade Kingsford 2032</x:t>
   </x:si>
   <x:si>
-    <x:t>210325.015004_Success</x:t>
+    <x:t>210329.035531_Success</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>